<commit_message>
add save record function
</commit_message>
<xml_diff>
--- a/db/patient_data.xlsx
+++ b/db/patient_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,12 +512,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Heru</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>11</v>
-      </c>
+          <t>MACHRUP, TN</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>HEAD</t>
@@ -525,38 +523,32 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>20180209</t>
+          <t>20150128</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>M</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J2" t="n">
-        <v>17.26</v>
-      </c>
-      <c r="K2" t="n">
-        <v>9.66</v>
-      </c>
+        <v>17.2908822613249</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
-        <v>100</v>
-      </c>
-      <c r="M2" t="n">
-        <v>96.8</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.54</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -564,155 +556,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Isabella</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>11</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>HEAD</t>
-        </is>
-      </c>
+          <t>XXXXXX-001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>20181031</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>21</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
+          <t>20170209</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J3" t="n">
-        <v>17.26</v>
-      </c>
-      <c r="K3" t="n">
-        <v>9.66</v>
-      </c>
+        <v>15.61301197983761</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
-        <v>100</v>
-      </c>
-      <c r="M3" t="n">
-        <v>96.8</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Bagaskara</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>HEAD</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>20180209</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>29</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" t="n">
-        <v>17.26</v>
-      </c>
-      <c r="K4" t="n">
-        <v>9.66</v>
-      </c>
-      <c r="L4" t="n">
-        <v>100</v>
-      </c>
-      <c r="M4" t="n">
-        <v>96.8</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mayang</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>11</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>HEAD</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>20181031</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>21</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" t="n">
-        <v>17.26</v>
-      </c>
-      <c r="K5" t="n">
-        <v>9.66</v>
-      </c>
-      <c r="L5" t="n">
-        <v>100</v>
-      </c>
-      <c r="M5" t="n">
-        <v>96.8</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.54</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>